<commit_message>
Fixes external gate sums
</commit_message>
<xml_diff>
--- a/docs/data/1_Targets_FromStreetlightData.xlsx
+++ b/docs/data/1_Targets_FromStreetlightData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC71AB62-1C38-47E5-8D9C-09626574E539}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D844EB6-916A-4E68-8823-75A98A7C9CD3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="838" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="838" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EI_IE_WorkTrips" sheetId="1" r:id="rId1"/>
@@ -421,7 +421,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
-    <numFmt numFmtId="168" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -753,20 +753,20 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1066,17 +1066,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
     </row>
     <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -1390,17 +1390,17 @@
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="54" t="s">
+      <c r="B12" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="54"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="59"/>
+      <c r="J12" s="59"/>
     </row>
     <row r="13" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
@@ -1704,17 +1704,17 @@
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="54" t="s">
+      <c r="B25" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="54"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="54"/>
-      <c r="I25" s="54"/>
-      <c r="J25" s="54"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="59"/>
     </row>
     <row r="26" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
@@ -2102,17 +2102,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="J2" s="59"/>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -2419,17 +2419,17 @@
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="54" t="s">
+      <c r="B12" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="54"/>
-      <c r="D12" s="54"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="54"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="59"/>
+      <c r="J12" s="59"/>
     </row>
     <row r="13" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
@@ -3296,34 +3296,34 @@
       </c>
     </row>
     <row r="11" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="55" t="s">
+      <c r="B11" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="55"/>
-      <c r="L11" s="56"/>
-      <c r="M11" s="57" t="s">
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="60"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="N11" s="57"/>
-      <c r="O11" s="57"/>
-      <c r="P11" s="57"/>
-      <c r="Q11" s="57"/>
-      <c r="R11" s="57"/>
-      <c r="S11" s="57"/>
-      <c r="V11" s="55" t="s">
+      <c r="N11" s="61"/>
+      <c r="O11" s="61"/>
+      <c r="P11" s="61"/>
+      <c r="Q11" s="61"/>
+      <c r="R11" s="61"/>
+      <c r="S11" s="61"/>
+      <c r="V11" s="60" t="s">
         <v>113</v>
       </c>
-      <c r="W11" s="55"/>
-      <c r="X11" s="55"/>
-      <c r="Y11" s="55"/>
-      <c r="Z11" s="55"/>
-      <c r="AA11" s="55"/>
-      <c r="AB11" s="55"/>
+      <c r="W11" s="60"/>
+      <c r="X11" s="60"/>
+      <c r="Y11" s="60"/>
+      <c r="Z11" s="60"/>
+      <c r="AA11" s="60"/>
+      <c r="AB11" s="60"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -3350,28 +3350,28 @@
       <c r="H12" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="L12" s="56" t="s">
+      <c r="L12" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="M12" s="58" t="s">
+      <c r="M12" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="N12" s="58" t="s">
+      <c r="N12" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="O12" s="58" t="s">
+      <c r="O12" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="P12" s="58" t="s">
+      <c r="P12" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="Q12" s="58" t="s">
+      <c r="Q12" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="R12" s="58" t="s">
+      <c r="R12" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="S12" s="58" t="s">
+      <c r="S12" s="55" t="s">
         <v>37</v>
       </c>
       <c r="U12" t="s">
@@ -3424,32 +3424,32 @@
       <c r="J13">
         <v>25.1</v>
       </c>
-      <c r="L13" s="59" t="s">
+      <c r="L13" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="M13" s="56"/>
-      <c r="N13" s="56">
+      <c r="M13" s="54"/>
+      <c r="N13" s="54">
         <f t="shared" ref="N13:N19" si="2">+C13-$J13</f>
         <v>41.9</v>
       </c>
-      <c r="O13" s="56">
+      <c r="O13" s="54">
         <f t="shared" ref="O13:O19" si="3">+D13-$J13</f>
         <v>51.6</v>
       </c>
-      <c r="P13" s="56">
+      <c r="P13" s="54">
         <f t="shared" ref="P13:P19" si="4">+E13-$J13</f>
         <v>66.900000000000006</v>
       </c>
-      <c r="Q13" s="56">
+      <c r="Q13" s="54">
         <f t="shared" ref="Q13:Q19" si="5">+F13-$J13</f>
         <v>76.900000000000006</v>
       </c>
-      <c r="R13" s="56">
+      <c r="R13" s="54">
         <f t="shared" ref="R13:R19" si="6">+G13-$J13</f>
         <v>44.499999999999993</v>
       </c>
-      <c r="S13" s="56">
-        <f t="shared" ref="S13:S19" si="7">+H13-$J13</f>
+      <c r="S13" s="54">
+        <f t="shared" ref="S13:S18" si="7">+H13-$J13</f>
         <v>31</v>
       </c>
       <c r="U13" s="15" t="s">
@@ -3476,7 +3476,7 @@
         <v>25.499999999999993</v>
       </c>
       <c r="AB13">
-        <f t="shared" ref="AB13:AB19" si="13">+S13-S$21</f>
+        <f t="shared" ref="AB13:AB18" si="13">+S13-S$21</f>
         <v>15.9</v>
       </c>
     </row>
@@ -3505,31 +3505,31 @@
       <c r="J14">
         <v>21.6</v>
       </c>
-      <c r="L14" s="59" t="s">
+      <c r="L14" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="M14" s="60">
+      <c r="M14" s="57">
         <f t="shared" ref="M14:M19" si="14">+B14-$J14</f>
         <v>45.4</v>
       </c>
-      <c r="N14" s="56"/>
-      <c r="O14" s="56">
+      <c r="N14" s="54"/>
+      <c r="O14" s="54">
         <f t="shared" si="3"/>
         <v>34.5</v>
       </c>
-      <c r="P14" s="56">
+      <c r="P14" s="54">
         <f t="shared" si="4"/>
         <v>49.800000000000004</v>
       </c>
-      <c r="Q14" s="56">
+      <c r="Q14" s="54">
         <f t="shared" si="5"/>
         <v>59.4</v>
       </c>
-      <c r="R14" s="56">
+      <c r="R14" s="54">
         <f t="shared" si="6"/>
         <v>51.499999999999993</v>
       </c>
-      <c r="S14" s="56">
+      <c r="S14" s="54">
         <f t="shared" si="7"/>
         <v>38.1</v>
       </c>
@@ -3586,31 +3586,31 @@
       <c r="J15">
         <v>17.2</v>
       </c>
-      <c r="L15" s="59" t="s">
+      <c r="L15" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="M15" s="56">
+      <c r="M15" s="54">
         <f t="shared" si="14"/>
         <v>59.5</v>
       </c>
-      <c r="N15" s="56">
+      <c r="N15" s="54">
         <f t="shared" si="2"/>
         <v>38.900000000000006</v>
       </c>
-      <c r="O15" s="56"/>
-      <c r="P15" s="56">
+      <c r="O15" s="54"/>
+      <c r="P15" s="54">
         <f t="shared" si="4"/>
         <v>40.5</v>
       </c>
-      <c r="Q15" s="56">
+      <c r="Q15" s="54">
         <f t="shared" si="5"/>
         <v>50.099999999999994</v>
       </c>
-      <c r="R15" s="56">
+      <c r="R15" s="54">
         <f t="shared" si="6"/>
         <v>60.2</v>
       </c>
-      <c r="S15" s="56">
+      <c r="S15" s="54">
         <f t="shared" si="7"/>
         <v>52.2</v>
       </c>
@@ -3667,31 +3667,31 @@
       <c r="J16">
         <v>16.7</v>
       </c>
-      <c r="L16" s="59" t="s">
+      <c r="L16" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="M16" s="56">
+      <c r="M16" s="54">
         <f t="shared" si="14"/>
         <v>75.3</v>
       </c>
-      <c r="N16" s="56">
+      <c r="N16" s="54">
         <f t="shared" si="2"/>
         <v>54.7</v>
       </c>
-      <c r="O16" s="56">
+      <c r="O16" s="54">
         <f t="shared" si="3"/>
         <v>41</v>
       </c>
-      <c r="P16" s="56"/>
-      <c r="Q16" s="56">
+      <c r="P16" s="54"/>
+      <c r="Q16" s="54">
         <f t="shared" si="5"/>
         <v>44.900000000000006</v>
       </c>
-      <c r="R16" s="56">
+      <c r="R16" s="54">
         <f t="shared" si="6"/>
         <v>64.7</v>
       </c>
-      <c r="S16" s="56">
+      <c r="S16" s="54">
         <f t="shared" si="7"/>
         <v>67.899999999999991</v>
       </c>
@@ -3748,31 +3748,31 @@
       <c r="J17">
         <v>30.9</v>
       </c>
-      <c r="L17" s="59" t="s">
+      <c r="L17" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="M17" s="60">
+      <c r="M17" s="57">
         <f t="shared" si="14"/>
         <v>71.099999999999994</v>
       </c>
-      <c r="N17" s="56">
+      <c r="N17" s="54">
         <f t="shared" si="2"/>
         <v>50.1</v>
       </c>
-      <c r="O17" s="56">
+      <c r="O17" s="54">
         <f t="shared" si="3"/>
         <v>36.4</v>
       </c>
-      <c r="P17" s="56">
+      <c r="P17" s="54">
         <f t="shared" si="4"/>
         <v>30.700000000000003</v>
       </c>
-      <c r="Q17" s="56"/>
-      <c r="R17" s="56">
+      <c r="Q17" s="54"/>
+      <c r="R17" s="54">
         <f t="shared" si="6"/>
         <v>60.199999999999996</v>
       </c>
-      <c r="S17" s="56">
+      <c r="S17" s="54">
         <f t="shared" si="7"/>
         <v>63.4</v>
       </c>
@@ -3829,31 +3829,31 @@
       <c r="J18">
         <v>19</v>
       </c>
-      <c r="L18" s="59" t="s">
+      <c r="L18" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="M18" s="56">
+      <c r="M18" s="54">
         <f t="shared" si="14"/>
         <v>50.599999999999994</v>
       </c>
-      <c r="N18" s="56">
+      <c r="N18" s="54">
         <f t="shared" si="2"/>
         <v>54.099999999999994</v>
       </c>
-      <c r="O18" s="56">
+      <c r="O18" s="54">
         <f t="shared" si="3"/>
         <v>58.400000000000006</v>
       </c>
-      <c r="P18" s="56">
+      <c r="P18" s="54">
         <f t="shared" si="4"/>
         <v>62.400000000000006</v>
       </c>
-      <c r="Q18" s="56">
+      <c r="Q18" s="54">
         <f t="shared" si="5"/>
         <v>72.099999999999994</v>
       </c>
-      <c r="R18" s="56"/>
-      <c r="S18" s="60">
+      <c r="R18" s="54"/>
+      <c r="S18" s="57">
         <f t="shared" si="7"/>
         <v>32.799999999999997</v>
       </c>
@@ -3910,34 +3910,34 @@
       <c r="J19">
         <v>15.1</v>
       </c>
-      <c r="L19" s="59" t="s">
+      <c r="L19" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="M19" s="56">
+      <c r="M19" s="54">
         <f t="shared" si="14"/>
         <v>41</v>
       </c>
-      <c r="N19" s="56">
+      <c r="N19" s="54">
         <f t="shared" si="2"/>
         <v>44.6</v>
       </c>
-      <c r="O19" s="56">
+      <c r="O19" s="54">
         <f t="shared" si="3"/>
         <v>54.300000000000004</v>
       </c>
-      <c r="P19" s="56">
+      <c r="P19" s="54">
         <f t="shared" si="4"/>
         <v>69.5</v>
       </c>
-      <c r="Q19" s="56">
+      <c r="Q19" s="54">
         <f t="shared" si="5"/>
         <v>79.2</v>
       </c>
-      <c r="R19" s="56">
+      <c r="R19" s="54">
         <f t="shared" si="6"/>
         <v>36.699999999999996</v>
       </c>
-      <c r="S19" s="56"/>
+      <c r="S19" s="54"/>
       <c r="U19" s="15" t="s">
         <v>37</v>
       </c>
@@ -3967,36 +3967,36 @@
       </c>
     </row>
     <row r="20" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="L20" s="56"/>
-      <c r="M20" s="56"/>
-      <c r="N20" s="56"/>
-      <c r="O20" s="56"/>
-      <c r="P20" s="56"/>
-      <c r="Q20" s="56"/>
-      <c r="R20" s="56"/>
-      <c r="S20" s="56"/>
+      <c r="L20" s="54"/>
+      <c r="M20" s="54"/>
+      <c r="N20" s="54"/>
+      <c r="O20" s="54"/>
+      <c r="P20" s="54"/>
+      <c r="Q20" s="54"/>
+      <c r="R20" s="54"/>
+      <c r="S20" s="54"/>
     </row>
     <row r="21" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L21" s="56"/>
-      <c r="M21" s="56">
+      <c r="L21" s="54"/>
+      <c r="M21" s="54">
         <v>25.1</v>
       </c>
-      <c r="N21" s="56">
+      <c r="N21" s="54">
         <v>21.6</v>
       </c>
-      <c r="O21" s="56">
+      <c r="O21" s="54">
         <v>17.2</v>
       </c>
-      <c r="P21" s="56">
+      <c r="P21" s="54">
         <v>16.7</v>
       </c>
-      <c r="Q21" s="56">
+      <c r="Q21" s="54">
         <v>30.9</v>
       </c>
-      <c r="R21" s="56">
+      <c r="R21" s="54">
         <v>19</v>
       </c>
-      <c r="S21" s="56">
+      <c r="S21" s="54">
         <v>15.1</v>
       </c>
     </row>
@@ -4633,7 +4633,7 @@
       </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="AD31" s="61">
+      <c r="AD31" s="58">
         <f>+AC30/I30</f>
         <v>0.32682469194900221</v>
       </c>
@@ -4653,8 +4653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17F4995B-D056-4A5F-8DDB-D0567BFDB8AB}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4734,8 +4734,8 @@
         <v>625.31075548939339</v>
       </c>
       <c r="H4" s="30">
-        <f t="shared" ref="H4:H10" si="2">I4-SUM(E4:G4)</f>
-        <v>3991.3602065500563</v>
+        <f>I4-SUM(D4:G4)</f>
+        <v>3102.3602065500563</v>
       </c>
       <c r="I4" s="26">
         <v>6849</v>
@@ -4766,8 +4766,8 @@
         <v>1351.9951618905843</v>
       </c>
       <c r="H5" s="30">
-        <f t="shared" si="2"/>
-        <v>8423.6664728321557</v>
+        <f t="shared" ref="H5:H10" si="2">I5-SUM(D5:G5)</f>
+        <v>6707.6664728321548</v>
       </c>
       <c r="I5" s="26">
         <v>14859</v>
@@ -4799,7 +4799,7 @@
       </c>
       <c r="H6" s="30">
         <f t="shared" si="2"/>
-        <v>3400.7552335318196</v>
+        <v>2679.7552335318201</v>
       </c>
       <c r="I6" s="26">
         <v>5743</v>
@@ -4831,7 +4831,7 @@
       </c>
       <c r="H7" s="30">
         <f t="shared" si="2"/>
-        <v>1018.7012467435803</v>
+        <v>591.70124674358021</v>
       </c>
       <c r="I7" s="26">
         <v>1887</v>
@@ -4863,7 +4863,7 @@
       </c>
       <c r="H8" s="30">
         <f t="shared" si="2"/>
-        <v>3306.8506698920728</v>
+        <v>2886.8506698920728</v>
       </c>
       <c r="I8" s="26">
         <v>6468</v>
@@ -4895,7 +4895,7 @@
       </c>
       <c r="H9" s="30">
         <f t="shared" si="2"/>
-        <v>5206.4337551172312</v>
+        <v>3654.4337551172312</v>
       </c>
       <c r="I9" s="26">
         <v>8413</v>
@@ -4927,7 +4927,7 @@
       </c>
       <c r="H10" s="30">
         <f t="shared" si="2"/>
-        <v>5124.2324153330856</v>
+        <v>3715.2324153330856</v>
       </c>
       <c r="I10" s="26">
         <v>8704</v>
@@ -5336,7 +5336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D72B3F2-04E7-424F-95D9-B0349C34D486}">
   <dimension ref="B2:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -5485,10 +5485,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="59" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="54"/>
+      <c r="D2" s="59"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -5705,10 +5705,10 @@
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C12" s="54" t="s">
+      <c r="C12" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="54"/>
+      <c r="D12" s="59"/>
       <c r="I12" t="s">
         <v>57</v>
       </c>
@@ -5894,10 +5894,10 @@
       <c r="D20">
         <v>2681</v>
       </c>
-      <c r="I20" s="54" t="s">
+      <c r="I20" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="J20" s="54"/>
+      <c r="J20" s="59"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="I21" t="s">
@@ -5908,10 +5908,10 @@
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C22" s="54" t="s">
+      <c r="C22" s="59" t="s">
         <v>88</v>
       </c>
-      <c r="D22" s="54"/>
+      <c r="D22" s="59"/>
       <c r="I22" t="s">
         <v>92</v>
       </c>

</xml_diff>